<commit_message>
[IMP] Adjust billing report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_billing.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_billing.xlsx
@@ -98,32 +98,27 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -187,25 +182,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -234,14 +237,14 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="28.06"/>
@@ -302,50 +305,50 @@
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMP] Adjust Purchase Billing Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_billing.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_billing.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">รายงานใบรับวางบิล</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">Purchase Billing Report</t>
   </si>
   <si>
     <t xml:space="preserve">Billing Date From</t>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Billing Due Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Billing Sent Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Supplier Code</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Document Due Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Receipt Date</t>
   </si>
   <si>
     <t xml:space="preserve">Billing Responsible</t>
@@ -95,8 +101,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -182,15 +190,31 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,8 +223,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -228,128 +260,140 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="28.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="27.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="30.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="32.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="36.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="4" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="11" t="s">
         <v>22</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] #2940 purchase billing report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_billing.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_billing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Purchase Billing Report</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">Billing Sent Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Billing Responsible</t>
+  </si>
+  <si>
     <t xml:space="preserve">Supplier Code</t>
   </si>
   <si>
@@ -91,7 +94,7 @@
     <t xml:space="preserve">Billing Receipt Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Billing Responsible</t>
+    <t xml:space="preserve">Invoice Responsible</t>
   </si>
   <si>
     <t xml:space="preserve">Document Status</t>
@@ -260,7 +263,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -272,20 +275,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="32.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="28.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="36.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="27.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="30.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="36.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="36.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="4" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,7 +309,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
@@ -316,7 +320,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
@@ -394,6 +398,9 @@
       </c>
       <c r="Q10" s="11" t="s">
         <v>24</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>